<commit_message>
manuscript, code, and data updates
</commit_message>
<xml_diff>
--- a/data/raw/ams_jena_template_2020-04-22/ams_jena_template.xlsx
+++ b/data/raw/ams_jena_template_2020-04-22/ams_jena_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>P-Nr.</t>
   </si>
@@ -635,6 +635,9 @@
   </si>
   <si>
     <t>single measurements of the respective sample, plus a contribution from the calibration by the standards</t>
+  </si>
+  <si>
+    <t>chr</t>
   </si>
 </sst>
 </file>
@@ -1159,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1472,13 +1475,27 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
+      <c r="A28" s="10">
+        <v>1</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="11">
+        <v>1</v>
+      </c>
+      <c r="D28" s="11">
+        <v>1</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="15">
       <c r="A29" s="10"/>

</xml_diff>